<commit_message>
adjusted report spreadsheets, matching now works for 85 cases, 6 of which are duplicated making for 91 rows
</commit_message>
<xml_diff>
--- a/PPO/intermediary_data/ciri_names.xlsx
+++ b/PPO/intermediary_data/ciri_names.xlsx
@@ -12,14 +12,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="266">
   <si>
     <t>.id</t>
   </si>
   <si>
-    <t>X.</t>
-  </si>
-  <si>
     <t>Voornaam</t>
   </si>
   <si>
@@ -303,276 +300,6 @@
   </si>
   <si>
     <t>WerktuigPPO |  June</t>
-  </si>
-  <si>
-    <t>24umpxnobj7z59xnl248ycq0g10hplsr</t>
-  </si>
-  <si>
-    <t>nstrndpsdls1mruhucknstrnfcpkp9q2</t>
-  </si>
-  <si>
-    <t>k1fh1u3pdyvworgnxtjlk1fhtg963dc4</t>
-  </si>
-  <si>
-    <t>vq8c05b78r98hmxjubrvyvq8c05b7xya</t>
-  </si>
-  <si>
-    <t>rfidzvjl7pur4so1rfidzg6djc872pc7</t>
-  </si>
-  <si>
-    <t>ksfhdljkzngtd6b9rd94ksfhdl8wcnl3</t>
-  </si>
-  <si>
-    <t>zei4i0k63doqtwaxuruzei4i0hfvgc2c</t>
-  </si>
-  <si>
-    <t>vfjscwi5iro50xbb5vfjscw5a4soawdy</t>
-  </si>
-  <si>
-    <t>lj2cxh04or887mlejc1lj2cxz7a1a3k8</t>
-  </si>
-  <si>
-    <t>voo8fs3rcv53ce1b9bvoo8mky3sxyxix</t>
-  </si>
-  <si>
-    <t>tlj01ng3uy4p1tlj0mzkhw62bnketkdw</t>
-  </si>
-  <si>
-    <t>90lopfvzeq2psulha3u90lopfvk1w8qy</t>
-  </si>
-  <si>
-    <t>z9vvya14r67btg8yz9v030os4dv9c9kl</t>
-  </si>
-  <si>
-    <t>43f0f81pvgyk43i39d9fw4zdpjj60uue</t>
-  </si>
-  <si>
-    <t>m5de6stvjtzhxm9ahm5d2c33t7cr40wb</t>
-  </si>
-  <si>
-    <t>hn6w5ndzgw3c3hbaxhn6w5nj15w50q63</t>
-  </si>
-  <si>
-    <t>41r0di8y9yig51d22k41r0di87vni4ln</t>
-  </si>
-  <si>
-    <t>n25pkyh5nx6be54zlul6n25pkyt58uks</t>
-  </si>
-  <si>
-    <t>tncs19dzwxibhb845p2r8tncs19hifyx</t>
-  </si>
-  <si>
-    <t>7auv3dp1zvxmokjfohs67auv3dpnch5h</t>
-  </si>
-  <si>
-    <t>6tpwwxhkbkr9gcfz06tpwh2t2qe4f9vf</t>
-  </si>
-  <si>
-    <t>vn0sov5u16lubh67obo4noevn0sov5u2</t>
-  </si>
-  <si>
-    <t>lbnavm1g45q2n6flbnav06usje973c1d</t>
-  </si>
-  <si>
-    <t>0vcgmbia00kn5buhv0vcb5492l44oswe</t>
-  </si>
-  <si>
-    <t>ksfxsyh18h9knkwhatboksfxsy1a4ier</t>
-  </si>
-  <si>
-    <t>hzvf49g1a58e7vzrb2hzvf4p1odypzo5</t>
-  </si>
-  <si>
-    <t>nswza4edh14tu7inswzaffc8uxabingi</t>
-  </si>
-  <si>
-    <t>k8zjf5977uaw7x3tmok8zjf594l5gqb8</t>
-  </si>
-  <si>
-    <t>8z8jvfnu0a0ygi2zwhhc1m8z8jvfnv5l</t>
-  </si>
-  <si>
-    <t>84tne70ztvbzumoi84tnektxhsc8gl6u</t>
-  </si>
-  <si>
-    <t>fchz1rt5aaea7h1e10byfchz1rttmb32</t>
-  </si>
-  <si>
-    <t>bi7o17txuvkkjf51kdbi7o1dd3bvwxxq</t>
-  </si>
-  <si>
-    <t>2y7na7usqmixsf4opsmw62y7n092opc5</t>
-  </si>
-  <si>
-    <t>ywcelf7o4osxivp6ib8qywcelyz54o46</t>
-  </si>
-  <si>
-    <t>nz7xzh6f3we6x6abql4twnz7xzh601av</t>
-  </si>
-  <si>
-    <t>fth5kjcvuwzzxh3vsq20qw8fth5kjccf</t>
-  </si>
-  <si>
-    <t>zs52eabhlv467mxxm3kixqu8plzs52ea</t>
-  </si>
-  <si>
-    <t>89iq7dne6nvfjd7tzs89iq7dniiijhpy</t>
-  </si>
-  <si>
-    <t>1hz8emin4zxm5s2f1hz8emikmkclogt8</t>
-  </si>
-  <si>
-    <t>zqhrpsqh8rhyb5synzqhrpsrp3amola6</t>
-  </si>
-  <si>
-    <t>9hkjll4acelq9js1oc3zai9hkjll4npk</t>
-  </si>
-  <si>
-    <t>y6hkn7ewxavb3e6mny6hkn1ey92q8wne</t>
-  </si>
-  <si>
-    <t>z07940zp2eg06ypkz07945bptx6fggv0</t>
-  </si>
-  <si>
-    <t>5w4tezkeacdi6lb5w4tcjxa342qoows3</t>
-  </si>
-  <si>
-    <t>yuagwijkksy69r96kb8s9yuagwijsw8a</t>
-  </si>
-  <si>
-    <t>yp9vas2hjoxriohyp9vatkc1y0v3lpa6</t>
-  </si>
-  <si>
-    <t>l03pztbj1mctpl03pvsnxp77ahm9v50d</t>
-  </si>
-  <si>
-    <t>r6niru6ltzwnye07n04d6r6nirl9rl9t</t>
-  </si>
-  <si>
-    <t>f2xsvfez7okhptf2xv6p2zh3bcnxh81b</t>
-  </si>
-  <si>
-    <t>0ddieri59ty49bpzazuk3mfg0ddieri5</t>
-  </si>
-  <si>
-    <t>b1s1ygc54bdy4didxxhb1s1yggl4keaa</t>
-  </si>
-  <si>
-    <t>mbnvo834qcuqkgplejmbnvov1gw80e4y</t>
-  </si>
-  <si>
-    <t>m9u3k0m0qhy87lk85icvqwm9u3k0m0ib</t>
-  </si>
-  <si>
-    <t>nl22mprudt6evgoqnl2laqftygkazc3m</t>
-  </si>
-  <si>
-    <t>esejsolg5jrnkesejm8af1ktinbpgoxu</t>
-  </si>
-  <si>
-    <t>7qpyztzqy3nvr7dcf627qpyztzqmqi0l</t>
-  </si>
-  <si>
-    <t>xa43rsblgwhruycfuafxa43rs213oykn</t>
-  </si>
-  <si>
-    <t>sbf30utr0trwah0v9rysbf3uwn8ovqdk</t>
-  </si>
-  <si>
-    <t>8bm2auc7xd4th8zgefj68bm2auc7uavf</t>
-  </si>
-  <si>
-    <t>y3qrf6kgytd9n08y3qreo79aahusz1ax</t>
-  </si>
-  <si>
-    <t>vprpu1kmb7t8ui04vb74eovprpu12jsp</t>
-  </si>
-  <si>
-    <t>swzktuh58e65qlwswzktf7i18fynafeb</t>
-  </si>
-  <si>
-    <t>62csk6ou3q4jucbjmwet62csk6yzi8rr</t>
-  </si>
-  <si>
-    <t>3zk4suwgfehmkp0yjy74l3zk4sufgqpp</t>
-  </si>
-  <si>
-    <t>i43lwiko6dix2i43lsrypagox2esrvme</t>
-  </si>
-  <si>
-    <t>fi5o9rh4kj862yssfi5o9ua2mgm1o99r</t>
-  </si>
-  <si>
-    <t>wqsrcdc9s376erfn7rfeurwqsrcdhnod</t>
-  </si>
-  <si>
-    <t>anhmw7r6gs3c10dadlwtanhmwj79a0l0</t>
-  </si>
-  <si>
-    <t>1qag0dkqt7fbb1xiuloa4fkq3lyaexiu</t>
-  </si>
-  <si>
-    <t>ihgal136vqdk0tq2p2wvcihgal04ose8</t>
-  </si>
-  <si>
-    <t>8fhsk8x3a0j8fm18fhsk8xw5lkcunxik</t>
-  </si>
-  <si>
-    <t>j837vgya7kfyg6hdx5j837vgv3b77dy0</t>
-  </si>
-  <si>
-    <t>k6woj5oo3d0pcoeu0qugevh2k6wobhm1</t>
-  </si>
-  <si>
-    <t>a130g4kaax6c7jd7a130noq9bgc4od87</t>
-  </si>
-  <si>
-    <t>hd748l2i3dhx1guqx3o6ghd748l2ylyj</t>
-  </si>
-  <si>
-    <t>an7trawezwexx49m8tp6an7trah7ms77</t>
-  </si>
-  <si>
-    <t>rtph6np59vmrsmrsmrtph6n09n1ofokr</t>
-  </si>
-  <si>
-    <t>92okz7iem7vnj7s7icv92iba4i5uqng3</t>
-  </si>
-  <si>
-    <t>srek42in9x1l6rndesrek99ooitwqz09</t>
-  </si>
-  <si>
-    <t>hh2mrx39na4sd0dl0e8r3hh2mlua71fd</t>
-  </si>
-  <si>
-    <t>s8y1yag55lvx0s1pks8y1uywxzxvi0tw</t>
-  </si>
-  <si>
-    <t>qjeod6216fuqp68yh9qjeod6gvxydrpm</t>
-  </si>
-  <si>
-    <t>vy9wa3u4zpoc9gkivy9828jb3n0wl6j7</t>
-  </si>
-  <si>
-    <t>g31dnmr9bi0y2r8ha7ag31dnmusiuzs5</t>
-  </si>
-  <si>
-    <t>mm7t87nkbvhhx58e82mm7t87naaqo74c</t>
-  </si>
-  <si>
-    <t>qjw543sd1r7mt9pzkqlhqjw543blbo7z</t>
-  </si>
-  <si>
-    <t>ivrhy9rrcan1a8kcvcmivrhy9rclpqdy</t>
-  </si>
-  <si>
-    <t>al6hrly6xlf0af23al6hr0mnx1dy4b2t</t>
-  </si>
-  <si>
-    <t>nr1166kfazgiwzkucs4k2nr1166wdr7r</t>
-  </si>
-  <si>
-    <t>fnndspun5aa7izr3cv2fnndsp59i0dmq</t>
   </si>
   <si>
     <t>carolien</t>
@@ -1144,1538 +871,1265 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E2" t="s">
-        <v>272</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" t="s">
-        <v>273</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E4" t="s">
-        <v>274</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E5" t="s">
-        <v>275</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" t="s">
-        <v>240</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
-      </c>
-      <c r="E7" t="s">
-        <v>276</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E8" t="s">
-        <v>277</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" t="s">
-        <v>278</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
-        <v>195</v>
-      </c>
-      <c r="E10" t="s">
-        <v>240</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>196</v>
-      </c>
-      <c r="E11" t="s">
-        <v>279</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>197</v>
-      </c>
-      <c r="E12" t="s">
-        <v>280</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>198</v>
-      </c>
-      <c r="E13" t="s">
-        <v>281</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>199</v>
-      </c>
-      <c r="E14" t="s">
-        <v>282</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
-      </c>
-      <c r="E15" t="s">
-        <v>283</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
-      </c>
-      <c r="E16" t="s">
-        <v>284</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E17" t="s">
-        <v>285</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" t="s">
-        <v>203</v>
-      </c>
-      <c r="E18" t="s">
-        <v>286</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
-        <v>204</v>
-      </c>
-      <c r="E19" t="s">
-        <v>287</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
-        <v>205</v>
-      </c>
-      <c r="E20" t="s">
-        <v>288</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D21" t="s">
-        <v>206</v>
-      </c>
-      <c r="E21" t="s">
-        <v>289</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
-      </c>
-      <c r="E22" t="s">
-        <v>290</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D23" t="s">
-        <v>207</v>
-      </c>
-      <c r="E23" t="s">
-        <v>291</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
-      </c>
-      <c r="E24" t="s">
-        <v>292</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>188</v>
-      </c>
-      <c r="E25" t="s">
-        <v>293</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>209</v>
-      </c>
-      <c r="E26" t="s">
-        <v>294</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>210</v>
-      </c>
-      <c r="E27" t="s">
-        <v>295</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>211</v>
-      </c>
-      <c r="E28" t="s">
-        <v>296</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>212</v>
-      </c>
-      <c r="E29" t="s">
-        <v>297</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>213</v>
-      </c>
-      <c r="E30" t="s">
-        <v>298</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D31" t="s">
-        <v>214</v>
-      </c>
-      <c r="E31" t="s">
-        <v>299</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D32" t="s">
-        <v>215</v>
-      </c>
-      <c r="E32" t="s">
-        <v>300</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D33" t="s">
-        <v>216</v>
-      </c>
-      <c r="E33" t="s">
-        <v>301</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D34" t="s">
-        <v>217</v>
-      </c>
-      <c r="E34" t="s">
-        <v>302</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D35" t="s">
-        <v>218</v>
-      </c>
-      <c r="E35" t="s">
-        <v>303</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D36" t="s">
-        <v>219</v>
-      </c>
-      <c r="E36" t="s">
-        <v>304</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D37" t="s">
-        <v>220</v>
-      </c>
-      <c r="E37" t="s">
-        <v>305</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D38" t="s">
-        <v>221</v>
-      </c>
-      <c r="E38" t="s">
-        <v>306</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>222</v>
-      </c>
-      <c r="E39" t="s">
-        <v>307</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>223</v>
-      </c>
-      <c r="E40" t="s">
-        <v>308</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" t="s">
-        <v>309</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D42" t="s">
-        <v>225</v>
-      </c>
-      <c r="E42" t="s">
-        <v>310</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D43" t="s">
-        <v>226</v>
-      </c>
-      <c r="E43" t="s">
-        <v>311</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D44" t="s">
-        <v>227</v>
-      </c>
-      <c r="E44" t="s">
-        <v>312</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D45" t="s">
-        <v>228</v>
-      </c>
-      <c r="E45" t="s">
-        <v>313</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
-        <v>229</v>
-      </c>
-      <c r="E46" t="s">
-        <v>314</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D47" t="s">
-        <v>230</v>
-      </c>
-      <c r="E47" t="s">
-        <v>315</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="D48" t="s">
-        <v>213</v>
-      </c>
-      <c r="E48" t="s">
-        <v>316</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D49" t="s">
-        <v>231</v>
-      </c>
-      <c r="E49" t="s">
-        <v>317</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D50" t="s">
-        <v>232</v>
-      </c>
-      <c r="E50" t="s">
-        <v>318</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>233</v>
-      </c>
-      <c r="E51" t="s">
-        <v>319</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D52" t="s">
-        <v>234</v>
-      </c>
-      <c r="E52" t="s">
-        <v>320</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D53" t="s">
-        <v>235</v>
-      </c>
-      <c r="E53" t="s">
-        <v>321</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D54" t="s">
-        <v>236</v>
-      </c>
-      <c r="E54" t="s">
-        <v>322</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D55" t="s">
-        <v>237</v>
-      </c>
-      <c r="E55" t="s">
-        <v>323</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D56" t="s">
-        <v>238</v>
-      </c>
-      <c r="E56" t="s">
-        <v>324</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>239</v>
-      </c>
-      <c r="E57" t="s">
-        <v>325</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>240</v>
-      </c>
-      <c r="E58" t="s">
-        <v>240</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C59" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D59" t="s">
-        <v>241</v>
-      </c>
-      <c r="E59" t="s">
-        <v>326</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C60" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D60" t="s">
-        <v>240</v>
-      </c>
-      <c r="E60" t="s">
-        <v>240</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D61" t="s">
-        <v>242</v>
-      </c>
-      <c r="E61" t="s">
-        <v>327</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D62" t="s">
-        <v>243</v>
-      </c>
-      <c r="E62" t="s">
-        <v>328</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C63" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D63" t="s">
-        <v>244</v>
-      </c>
-      <c r="E63" t="s">
-        <v>329</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C64" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D64" t="s">
-        <v>245</v>
-      </c>
-      <c r="E64" t="s">
-        <v>330</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C65" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D65" t="s">
-        <v>246</v>
-      </c>
-      <c r="E65" t="s">
-        <v>331</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D66" t="s">
-        <v>247</v>
-      </c>
-      <c r="E66" t="s">
-        <v>332</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C67" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D67" t="s">
-        <v>248</v>
-      </c>
-      <c r="E67" t="s">
-        <v>333</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C68" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D68" t="s">
-        <v>249</v>
-      </c>
-      <c r="E68" t="s">
-        <v>334</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C69" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D69" t="s">
-        <v>250</v>
-      </c>
-      <c r="E69" t="s">
-        <v>335</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C70" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D70" t="s">
-        <v>251</v>
-      </c>
-      <c r="E70" t="s">
-        <v>336</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C71" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D71" t="s">
-        <v>252</v>
-      </c>
-      <c r="E71" t="s">
-        <v>337</v>
+        <v>246</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C72" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D72" t="s">
-        <v>253</v>
-      </c>
-      <c r="E72" t="s">
-        <v>338</v>
+        <v>247</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D73" t="s">
-        <v>254</v>
-      </c>
-      <c r="E73" t="s">
-        <v>339</v>
+        <v>248</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D74" t="s">
-        <v>255</v>
-      </c>
-      <c r="E74" t="s">
-        <v>340</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D75" t="s">
-        <v>256</v>
-      </c>
-      <c r="E75" t="s">
-        <v>341</v>
+        <v>250</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D76" t="s">
-        <v>257</v>
-      </c>
-      <c r="E76" t="s">
-        <v>342</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D77" t="s">
-        <v>258</v>
-      </c>
-      <c r="E77" t="s">
-        <v>343</v>
+        <v>252</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C78" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D78" t="s">
-        <v>259</v>
-      </c>
-      <c r="E78" t="s">
-        <v>344</v>
+        <v>253</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C79" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D79" t="s">
-        <v>260</v>
-      </c>
-      <c r="E79" t="s">
-        <v>345</v>
+        <v>254</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D80" t="s">
-        <v>261</v>
-      </c>
-      <c r="E80" t="s">
-        <v>346</v>
+        <v>255</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C81" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D81" t="s">
-        <v>262</v>
-      </c>
-      <c r="E81" t="s">
-        <v>280</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="D82" t="s">
-        <v>217</v>
-      </c>
-      <c r="E82" t="s">
-        <v>347</v>
+        <v>256</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D83" t="s">
-        <v>263</v>
-      </c>
-      <c r="E83" t="s">
-        <v>348</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C84" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D84" t="s">
-        <v>264</v>
-      </c>
-      <c r="E84" t="s">
-        <v>349</v>
+        <v>258</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C85" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D85" t="s">
-        <v>265</v>
-      </c>
-      <c r="E85" t="s">
-        <v>350</v>
+        <v>259</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C86" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D86" t="s">
-        <v>266</v>
-      </c>
-      <c r="E86" t="s">
-        <v>351</v>
+        <v>260</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C87" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D87" t="s">
-        <v>267</v>
-      </c>
-      <c r="E87" t="s">
-        <v>352</v>
+        <v>261</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C88" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D88" t="s">
-        <v>268</v>
-      </c>
-      <c r="E88" t="s">
-        <v>353</v>
+        <v>262</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C89" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D89" t="s">
-        <v>269</v>
-      </c>
-      <c r="E89" t="s">
-        <v>354</v>
+        <v>263</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C90" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D90" t="s">
-        <v>270</v>
-      </c>
-      <c r="E90" t="s">
-        <v>355</v>
+        <v>264</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C91" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D91" t="s">
-        <v>271</v>
-      </c>
-      <c r="E91" t="s">
-        <v>356</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>